<commit_message>
first set (without substitution) complete
</commit_message>
<xml_diff>
--- a/New Language/Syntax Analyze Phase/FirstFollowSet/firstFollowSet.xlsx
+++ b/New Language/Syntax Analyze Phase/FirstFollowSet/firstFollowSet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="304">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -531,15 +531,6 @@
     <t xml:space="preserve">&lt;DIM_PASS&gt;     </t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;MUL_ARR_DEC&gt;  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;EMP_ARR_DEC&gt;  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;LEN_OF_ARR&gt;   </t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;ARR_CONST&gt;    </t>
   </si>
   <si>
@@ -576,9 +567,6 @@
     <t xml:space="preserve">&lt;EXPR&gt; ? ] </t>
   </si>
   <si>
-    <t> [ ? ;</t>
-  </si>
-  <si>
     <t>[ ? &lt;ARR_CONST&gt;</t>
   </si>
   <si>
@@ -589,13 +577,381 @@
   </si>
   <si>
     <t xml:space="preserve">, ? } </t>
+  </si>
+  <si>
+    <t>&lt;MUL_ARR_DEC2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;EMP_ARR_DEC2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;MUL_ARR_DEC&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LEN_OF_ARR&gt;</t>
+  </si>
+  <si>
+    <t>&lt;EMP_ARR_DEC&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LEN_OF_ARR2&gt;</t>
+  </si>
+  <si>
+    <t>[ ? ;</t>
+  </si>
+  <si>
+    <t>&lt;EXPR&gt;? ]</t>
+  </si>
+  <si>
+    <t>[? ;</t>
+  </si>
+  <si>
+    <t>Global Variable Declaration</t>
+  </si>
+  <si>
+    <t>&lt;GLOBAL_DEC&gt;</t>
+  </si>
+  <si>
+    <t>&lt;IS_FINAL_G&gt;</t>
+  </si>
+  <si>
+    <t>&lt;VAR_OBJ_G&gt;</t>
+  </si>
+  <si>
+    <t>&lt;VAR_ARR_G&gt;</t>
+  </si>
+  <si>
+    <t>&lt;IS_INIT_G&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LIST_G&gt;</t>
+  </si>
+  <si>
+    <t>const ? dt ? Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;TYPE&gt; </t>
+  </si>
+  <si>
+    <t>&lt;ARR_CLASS_DEC&gt; ? id &lt;IS_INIT_G&gt;</t>
+  </si>
+  <si>
+    <t>= &lt;INIT&gt; ? ;</t>
+  </si>
+  <si>
+    <t>, ?  ;</t>
+  </si>
+  <si>
+    <t>Attribute Declaration in class</t>
+  </si>
+  <si>
+    <t>&lt;ATTR_CLASS_DEC&gt;</t>
+  </si>
+  <si>
+    <t>&lt;IS_FINAL&gt;</t>
+  </si>
+  <si>
+    <t>&lt;VAR_OBJ_C&gt;</t>
+  </si>
+  <si>
+    <t>&lt;VAR_ARR_C&gt;</t>
+  </si>
+  <si>
+    <t>&lt;IS_INIT_C&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LIST_C&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">const ? dt ? id </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;ARR_CLASS_DEC&gt; ? &lt;ACCESSMOD&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">, ? ; </t>
+  </si>
+  <si>
+    <t>Expression(Right Recursive)</t>
+  </si>
+  <si>
+    <t>&lt;EXPR&gt;</t>
+  </si>
+  <si>
+    <t>&lt;EXPR1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;F&gt;</t>
+  </si>
+  <si>
+    <t>&lt;F1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;G&gt;</t>
+  </si>
+  <si>
+    <t>&lt;G1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;H&gt;</t>
+  </si>
+  <si>
+    <t>&lt;H1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;I&gt;</t>
+  </si>
+  <si>
+    <t>&lt;I1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;J&gt;</t>
+  </si>
+  <si>
+    <t>&lt;K&gt;</t>
+  </si>
+  <si>
+    <t>&lt;IS_FLAG&gt;</t>
+  </si>
+  <si>
+    <t>or ? null</t>
+  </si>
+  <si>
+    <t>and ? null</t>
+  </si>
+  <si>
+    <t>rop ?  null</t>
+  </si>
+  <si>
+    <t> pm ? null  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;J&gt; </t>
+  </si>
+  <si>
+    <t>mdm ? null</t>
+  </si>
+  <si>
+    <t>power ? null</t>
+  </si>
+  <si>
+    <t>&lt;FLAG&gt; ? &lt;OPERANDS&gt;</t>
+  </si>
+  <si>
+    <t>Operands</t>
+  </si>
+  <si>
+    <t>&lt;OPERAND&gt;</t>
+  </si>
+  <si>
+    <t>&lt;UNARY&gt;</t>
+  </si>
+  <si>
+    <t>&lt;FLAG&gt;</t>
+  </si>
+  <si>
+    <t>&lt;IS_ACMETH&gt;? &lt;INC_DEC&gt; ? ( ? &lt;UNARY&gt;
+? &lt;CONST&gt;</t>
+  </si>
+  <si>
+    <t>typeCast ? not</t>
+  </si>
+  <si>
+    <t>pm</t>
+  </si>
+  <si>
+    <t>Increment Decrement</t>
+  </si>
+  <si>
+    <t>&lt;CONST&gt;</t>
+  </si>
+  <si>
+    <t>intConst ? floatConst ? charConst ? 
+boolConst ? strConst</t>
+  </si>
+  <si>
+    <t>Conditional Statements</t>
+  </si>
+  <si>
+    <t>&lt;IF_ELSE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;OELSE&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if </t>
+  </si>
+  <si>
+    <t>else ? null</t>
+  </si>
+  <si>
+    <t>if-else</t>
+  </si>
+  <si>
+    <t>switch-case</t>
+  </si>
+  <si>
+    <t>&lt;SWITCH&gt;</t>
+  </si>
+  <si>
+    <t>&lt;STATE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;DEFAULT&gt;</t>
+  </si>
+  <si>
+    <t>&lt;TWO_MST&gt;</t>
+  </si>
+  <si>
+    <t>shift</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>state ? &lt;DEFAULT&gt; ? }</t>
+  </si>
+  <si>
+    <t>&lt;MST&gt; ? {</t>
+  </si>
+  <si>
+    <t>Loop Statements</t>
+  </si>
+  <si>
+    <t>Loop</t>
+  </si>
+  <si>
+    <t>While/do-while loop</t>
+  </si>
+  <si>
+    <t>&lt;LOOP&gt;</t>
+  </si>
+  <si>
+    <t>&lt;LT&gt;</t>
+  </si>
+  <si>
+    <t> loop</t>
+  </si>
+  <si>
+    <t>&lt;WHILE_ST&gt; ? &lt;FOR_ST&gt;</t>
+  </si>
+  <si>
+    <t>&lt;WHILE_ST&gt;</t>
+  </si>
+  <si>
+    <t>&lt;DO_WHILE&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">till </t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>For-loop</t>
+  </si>
+  <si>
+    <t>&lt;FOR_ST&gt;</t>
+  </si>
+  <si>
+    <t>&lt;FOR_ARG&gt;</t>
+  </si>
+  <si>
+    <t>&lt;POS3&gt;</t>
+  </si>
+  <si>
+    <t>&lt;DOT_ID5&gt;</t>
+  </si>
+  <si>
+    <t>thru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id? ( </t>
+  </si>
+  <si>
+    <t>&lt;DOT_ID5&gt; ? &lt;SUBSCRIPT&gt;? &lt;FN_BRACKETS&gt;</t>
+  </si>
+  <si>
+    <t> dot ? null</t>
+  </si>
+  <si>
+    <t>Jump Statements</t>
+  </si>
+  <si>
+    <t>Break-continue</t>
+  </si>
+  <si>
+    <t>Return-statement</t>
+  </si>
+  <si>
+    <t>&lt;BREAK&gt;</t>
+  </si>
+  <si>
+    <t>&lt;CONTINUE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;L&gt;</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t> cont</t>
+  </si>
+  <si>
+    <t>id ? ;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;RET_ST&gt; </t>
+  </si>
+  <si>
+    <t>ret</t>
+  </si>
+  <si>
+    <t>Throw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;THROW&gt; </t>
+  </si>
+  <si>
+    <t>raise</t>
+  </si>
+  <si>
+    <t>Exception Handler</t>
+  </si>
+  <si>
+    <t>&lt;TRY_CATCH&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ERROR_TYPE&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ERR_DOT&gt;</t>
+  </si>
+  <si>
+    <t>&lt;THROWS&gt;</t>
+  </si>
+  <si>
+    <t>&lt;FINALLY&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> test </t>
+  </si>
+  <si>
+    <t>dot ? id</t>
+  </si>
+  <si>
+    <t>raises ? null</t>
+  </si>
+  <si>
+    <t>finally ? null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,15 +974,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE1EFFF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -641,6 +1017,17 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -668,12 +1055,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -684,9 +1073,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -694,8 +1080,28 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="40% - Accent3" xfId="4" builtinId="39"/>
+    <cellStyle name="Accent3" xfId="3" builtinId="37"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -976,18 +1382,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D128"/>
+  <dimension ref="B1:D221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" x14ac:dyDescent="0.25">
@@ -1002,7 +1408,7 @@
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="14" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2"/>
@@ -1055,7 +1461,7 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="2"/>
@@ -1076,14 +1482,14 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1104,7 +1510,7 @@
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="14" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="2"/>
@@ -1125,7 +1531,7 @@
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C19" s="2"/>
@@ -1164,7 +1570,7 @@
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="14" t="s">
         <v>25</v>
       </c>
       <c r="C24" s="2"/>
@@ -1221,7 +1627,7 @@
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="14" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="2"/>
@@ -1260,7 +1666,7 @@
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C36" s="2"/>
@@ -1340,7 +1746,7 @@
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="2"/>
@@ -1402,7 +1808,7 @@
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C54" s="2"/>
@@ -1477,7 +1883,7 @@
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="14" t="s">
         <v>82</v>
       </c>
       <c r="C63" s="2"/>
@@ -1507,14 +1913,14 @@
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="14" t="s">
         <v>108</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="14" t="s">
         <v>87</v>
       </c>
       <c r="C68" s="2"/>
@@ -1589,7 +1995,7 @@
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="12" t="s">
         <v>100</v>
       </c>
       <c r="C77" s="2"/>
@@ -1628,14 +2034,14 @@
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="14" t="s">
         <v>107</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="12" t="s">
         <v>109</v>
       </c>
       <c r="C83" s="2"/>
@@ -1672,7 +2078,7 @@
       <c r="B87" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="C87" t="s">
         <v>127</v>
       </c>
       <c r="D87" s="2"/>
@@ -1681,7 +2087,7 @@
       <c r="B88" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C88" s="6" t="s">
+      <c r="C88" s="5" t="s">
         <v>128</v>
       </c>
       <c r="D88" s="2"/>
@@ -1762,7 +2168,7 @@
       <c r="B97" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C97" s="5" t="s">
         <v>137</v>
       </c>
       <c r="D97" s="2"/>
@@ -1773,14 +2179,14 @@
       <c r="D98" s="2"/>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="14" t="s">
         <v>138</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="12" t="s">
         <v>139</v>
       </c>
       <c r="C100" s="2"/>
@@ -1828,7 +2234,7 @@
       <c r="D105" s="2"/>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B106" s="4" t="s">
+      <c r="B106" s="14" t="s">
         <v>148</v>
       </c>
       <c r="C106" s="2"/>
@@ -1858,7 +2264,7 @@
       <c r="D109" s="2"/>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="14" t="s">
         <v>153</v>
       </c>
       <c r="C110" s="2"/>
@@ -1887,7 +2293,7 @@
         <v>156</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D113" s="2"/>
     </row>
@@ -1895,8 +2301,8 @@
       <c r="B114" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C114" s="6" t="s">
-        <v>173</v>
+      <c r="C114" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="D114" s="2"/>
     </row>
@@ -1905,7 +2311,7 @@
         <v>158</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D115" s="2"/>
     </row>
@@ -1914,7 +2320,7 @@
         <v>159</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D116" s="2"/>
     </row>
@@ -1923,7 +2329,7 @@
         <v>160</v>
       </c>
       <c r="C117" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
@@ -1931,7 +2337,7 @@
         <v>161</v>
       </c>
       <c r="C118" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
@@ -1947,15 +2353,15 @@
         <v>163</v>
       </c>
       <c r="C120" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>164</v>
       </c>
-      <c r="C121" s="7" t="s">
-        <v>179</v>
+      <c r="C121" s="6" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
@@ -1963,55 +2369,602 @@
         <v>165</v>
       </c>
       <c r="C122" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B123" t="s">
-        <v>166</v>
-      </c>
-      <c r="C123" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="C124" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
     </row>
     <row r="125" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="C125" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="126" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="C126" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="C127" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="128" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="C128" t="s">
-        <v>185</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>183</v>
+      </c>
+      <c r="C129" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>166</v>
+      </c>
+      <c r="C132" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>167</v>
+      </c>
+      <c r="C133" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>168</v>
+      </c>
+      <c r="C134" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135" s="7"/>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B136" s="11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>192</v>
+      </c>
+      <c r="C137" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>193</v>
+      </c>
+      <c r="C138" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>194</v>
+      </c>
+      <c r="C139" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>195</v>
+      </c>
+      <c r="C140" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>196</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>197</v>
+      </c>
+      <c r="C142" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B144" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>204</v>
+      </c>
+      <c r="C145" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>205</v>
+      </c>
+      <c r="C146" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>206</v>
+      </c>
+      <c r="C147" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>207</v>
+      </c>
+      <c r="C148" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>208</v>
+      </c>
+      <c r="C149" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>209</v>
+      </c>
+      <c r="C150" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B152" s="11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>214</v>
+      </c>
+      <c r="C153" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>215</v>
+      </c>
+      <c r="C154" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>216</v>
+      </c>
+      <c r="C155" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>217</v>
+      </c>
+      <c r="C156" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>218</v>
+      </c>
+      <c r="C157" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>219</v>
+      </c>
+      <c r="C158" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>220</v>
+      </c>
+      <c r="C159" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>221</v>
+      </c>
+      <c r="C160" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>222</v>
+      </c>
+      <c r="C161" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>223</v>
+      </c>
+      <c r="C162" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>224</v>
+      </c>
+      <c r="C163" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>135</v>
+      </c>
+      <c r="C164" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>225</v>
+      </c>
+      <c r="C165" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>226</v>
+      </c>
+      <c r="C166" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B168" s="11" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="169" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B169" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C169" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>237</v>
+      </c>
+      <c r="C170" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>238</v>
+      </c>
+      <c r="C171" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B173" s="11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B174" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C174" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B176" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B177" s="13" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
+        <v>246</v>
+      </c>
+      <c r="C178" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
+        <v>247</v>
+      </c>
+      <c r="C179" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B181" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B182" t="s">
+        <v>252</v>
+      </c>
+      <c r="C182" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
+        <v>253</v>
+      </c>
+      <c r="C183" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
+        <v>254</v>
+      </c>
+      <c r="C184" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B185" t="s">
+        <v>255</v>
+      </c>
+      <c r="C185" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B187" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B189" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
+        <v>263</v>
+      </c>
+      <c r="C190" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
+        <v>264</v>
+      </c>
+      <c r="C191" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B193" s="13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
+        <v>267</v>
+      </c>
+      <c r="C194" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>268</v>
+      </c>
+      <c r="C195" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B197" s="13" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>272</v>
+      </c>
+      <c r="C198" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>273</v>
+      </c>
+      <c r="C199" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
+        <v>274</v>
+      </c>
+      <c r="C200" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>275</v>
+      </c>
+      <c r="C201" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B203" s="11" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B204" s="8"/>
+    </row>
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B205" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B206" t="s">
+        <v>283</v>
+      </c>
+      <c r="C206" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
+        <v>284</v>
+      </c>
+      <c r="C207" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
+        <v>285</v>
+      </c>
+      <c r="C208" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B210" s="13" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>289</v>
+      </c>
+      <c r="C211" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B213" s="11" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>292</v>
+      </c>
+      <c r="C214" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B216" s="11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
+        <v>295</v>
+      </c>
+      <c r="C217" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>296</v>
+      </c>
+      <c r="C218" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>297</v>
+      </c>
+      <c r="C219" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>298</v>
+      </c>
+      <c r="C220" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
+        <v>299</v>
+      </c>
+      <c r="C221" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first set final push
</commit_message>
<xml_diff>
--- a/New Language/Syntax Analyze Phase/FirstFollowSet/firstFollowSet.xlsx
+++ b/New Language/Syntax Analyze Phase/FirstFollowSet/firstFollowSet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="363">
   <si>
     <t>&lt;Start&gt;</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>&lt;ACCESS_METH&gt;</t>
-  </si>
-  <si>
-    <t>dot?;</t>
   </si>
   <si>
     <t>&lt;SST&gt;?null</t>
@@ -374,10 +371,6 @@
     <t>&lt;ACCESS_METH&gt; ? null</t>
   </si>
   <si>
-    <t>&lt;INC_DEC&gt;? (? &lt;UNARY&gt; ?
-&lt;CONST&gt; ? &lt;FLAG&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;DOT_EXPR&gt; ? &lt;SUBSCRIPT&gt; ?&lt;FN_BRACKETS&gt; </t>
   </si>
   <si>
@@ -385,9 +378,6 @@
 &lt;NEW_OBJ&gt; ? &lt;ID_TO_EXPR&gt; </t>
   </si>
   <si>
-    <t>dot ? &lt;ID_TO_EXPR&gt; ? null</t>
-  </si>
-  <si>
     <t>&lt;J1&gt;</t>
   </si>
   <si>
@@ -496,18 +486,9 @@
     <t>= ? ;</t>
   </si>
   <si>
-    <t>&lt;REF_NEWARR&gt; ? &lt;NEW_ARR_CONST&gt;</t>
-  </si>
-  <si>
-    <t>new? &lt;DIM_PASS&gt;</t>
-  </si>
-  <si>
     <t>id ? &lt;NEW_ARR_CONST&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;DOT_ARR&gt;?&lt;SUBSCRIPT&gt; ? &lt;FN_BRACKETS&gt; </t>
-  </si>
-  <si>
     <t>&lt;DOT_ARR&gt; ? ;</t>
   </si>
   <si>
@@ -584,9 +565,6 @@
   </si>
   <si>
     <t>&lt;ARR_CLASS_DEC&gt; ? id &lt;IS_INIT_G&gt;</t>
-  </si>
-  <si>
-    <t>= &lt;INIT&gt; ? ;</t>
   </si>
   <si>
     <t>, ?  ;</t>
@@ -911,10 +889,6 @@
   </si>
   <si>
     <t>def ? Class ? Const ? Null</t>
-  </si>
-  <si>
-    <t>&lt;FN_DEC&gt; ? &lt;GLOBAL_CLASS&gt; ?
-&lt;GLOBAL_DEC&gt; ? null</t>
   </si>
   <si>
     <t>&lt;MAIN&gt; ? &lt;FN_DEC&gt; ? &lt;GLOBAL_CLASS&gt; ?
@@ -935,6 +909,9 @@
     <t>dt ? str</t>
   </si>
   <si>
+    <t>id | dt | str</t>
+  </si>
+  <si>
     <t>id? dt ? Str</t>
   </si>
   <si>
@@ -978,9 +955,6 @@
   </si>
   <si>
     <t>&lt;RET_OBJ_C&gt;</t>
-  </si>
-  <si>
-    <t>Static?dt ? str ? Id ? private ? Protected</t>
   </si>
   <si>
     <t>Static ? &lt;IS_FINAL&gt;</t>
@@ -1064,13 +1038,114 @@
   </si>
   <si>
     <t> dot ? Null ? [ ? (</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> till ? thru</t>
+  </si>
+  <si>
+    <t>[ ? protected ? Private ? Id</t>
+  </si>
+  <si>
+    <t>=  ? ;</t>
+  </si>
+  <si>
+    <t>( ? [</t>
+  </si>
+  <si>
+    <t>[ ? Id ? =  ? ;</t>
+  </si>
+  <si>
+    <t>pm ? parent ? Self ? id ? ( ? typeCast ? not? intConst ? 
+floatConst ? charConst ? boolConst ? strConst ? {  ? }</t>
+  </si>
+  <si>
+    <t>pm ? parent ? Self ? id ? ( ? typeCast ? not? intConst ? 
+floatConst ? charConst ? boolConst ? strConst ? ]</t>
+  </si>
+  <si>
+    <t>[ ? {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;DOT_ARR&gt;? &lt;SUBSCRIPT&gt; ? &lt;FN_BRACKETS&gt; </t>
+  </si>
+  <si>
+    <t>dot ? Null ? ;</t>
+  </si>
+  <si>
+    <t>dot ? = ? ;  ? [ ? (</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id ? new </t>
+  </si>
+  <si>
+    <t>&lt;FN_DEC&gt; ? &lt;GLOBAL_CLASS&gt; ?
+&lt;GLOBAL_DEC&gt; ? Null</t>
+  </si>
+  <si>
+    <t>&lt;ID_STAR&gt;</t>
+  </si>
+  <si>
+    <t>id ? power ? ;</t>
+  </si>
+  <si>
+    <t>dot ? ;</t>
+  </si>
+  <si>
+    <t>power ?  Mdm ?  Pm ? Rop ? And ? Or ? Null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dot ? &lt;ID_TO_EXPR&gt;  </t>
+  </si>
+  <si>
+    <t>dot ? = ? Cma ? ++ ? --? new? NaN ? power 
+?  Mdm ?  Pm ? Rop ? And ? Or ? Null</t>
+  </si>
+  <si>
+    <t>dot ? power ?  Mdm ?  Pm ? Rop ? And ? 
+Or ? Null</t>
+  </si>
+  <si>
+    <t>dot ? power ?  Mdm ?  Pm ? Rop ? And ? 
+Or ? Null ? [ ? (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;INC_DEC&gt;? (? &lt;UNARY&gt; ?
+&lt;CONST&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">++ ? --? ( ? typeCast ? Not ? intConst ? floatConst 
+? charConst ? boolConst ? strConst </t>
+  </si>
+  <si>
+    <t>parent ? Self ? id ? new? NaN ?  ++ ? --? ( ? typeCast 
+? Not ? intConst ? floatConst 
+? charConst ? boolConst ? strConst ? Pm</t>
+  </si>
+  <si>
+    <t>Static ?dt ? str ? Id ? private ? Protected</t>
+  </si>
+  <si>
+    <t>if ? Shift ? const ? dt ? id ? Parent ? Self ?  test?  Loop ? do ? stop ? Ret ? Cont ? raise</t>
+  </si>
+  <si>
+    <t>if ? Shift ? const ? dt ? id ? Parent ? Self ?  test?  Loop ? do ? stop ? Ret ? Cont ? Raise ? Null</t>
+  </si>
+  <si>
+    <t>; ?  if ? Shift ? const ? dt ? id ? Parent ? Self ?  
+test?  Loop ? do ? stop ? Ret ? Cont ? Raise ? {</t>
+  </si>
+  <si>
+    <t>if ? Shift ? const ? dt ? id ? Parent ? Self ?  test?  Loop ? do ? stop ? Ret ? Cont ? Raise ? Null ? {</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1081,13 +1156,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1121,7 +1189,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1131,11 +1199,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -1194,15 +1257,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1213,15 +1275,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1230,44 +1289,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="40% - Accent3" xfId="4" builtinId="39"/>
-    <cellStyle name="Accent3" xfId="3" builtinId="37"/>
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="5">
+    <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
+    <cellStyle name="Accent3" xfId="2" builtinId="37"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="5" builtinId="10"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1545,10 +1598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D224"/>
+  <dimension ref="B1:D225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B184" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C188" sqref="C188"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D195" sqref="D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,11 +1620,11 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="2"/>
@@ -1581,8 +1634,8 @@
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>289</v>
+      <c r="C3" s="15" t="s">
+        <v>282</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>20</v>
@@ -1592,7 +1645,7 @@
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1603,22 +1656,22 @@
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>294</v>
+      <c r="C5" s="16" t="s">
+        <v>286</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="18" t="s">
-        <v>293</v>
+      <c r="C6" s="16" t="s">
+        <v>346</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -1632,50 +1685,52 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="8" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
     </row>
     <row r="13" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>295</v>
-      </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="C13" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="4"/>
+      <c r="C14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
@@ -1683,7 +1738,7 @@
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="2"/>
@@ -1704,7 +1759,7 @@
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="2"/>
@@ -1733,91 +1788,95 @@
         <v>19</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>349</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>348</v>
+      </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
-        <v>22</v>
-      </c>
+      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>318</v>
-      </c>
+      <c r="B25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>30</v>
+        <v>290</v>
       </c>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>296</v>
+        <v>29</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D29" s="2"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>289</v>
+      </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
-        <v>31</v>
-      </c>
+      <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -1831,1422 +1890,1491 @@
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
-        <v>34</v>
-      </c>
+      <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="B37" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C41" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>302</v>
-      </c>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="17" t="s">
-        <v>300</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="B45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="14" t="s">
-        <v>47</v>
-      </c>
+      <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="B47" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>308</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>309</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="2"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>301</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>312</v>
+        <v>303</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C51" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B52" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="C52" s="18" t="s">
+      <c r="C54" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="14" t="s">
-        <v>55</v>
-      </c>
+      <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>305</v>
-      </c>
+      <c r="B56" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D57" t="s">
-        <v>319</v>
+        <v>55</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="D58" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>65</v>
+        <v>284</v>
       </c>
       <c r="D59" s="2"/>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
+      <c r="B63" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" s="14" t="s">
-        <v>68</v>
-      </c>
+      <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>316</v>
-      </c>
+      <c r="B65" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C66" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C66" s="17" t="s">
-        <v>72</v>
-      </c>
       <c r="D66" s="2" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
+      <c r="B67" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="14" t="s">
-        <v>92</v>
-      </c>
+      <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B69" s="14" t="s">
-        <v>73</v>
+      <c r="B69" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B70" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D71" s="2"/>
+        <v>73</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>306</v>
+        <v>74</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>307</v>
+        <v>29</v>
       </c>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B74" s="2" t="s">
+      <c r="C75" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C74" s="17" t="s">
+      <c r="C76" t="s">
+        <v>45</v>
+      </c>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D74" s="9" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B75" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C75" t="s">
-        <v>46</v>
-      </c>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B76" s="2" t="s">
+      <c r="D77" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="C78" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B79" s="15" t="s">
-        <v>287</v>
-      </c>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B80" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C80" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>331</v>
-      </c>
+    <row r="80" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B80" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="D81" s="5" t="s">
-        <v>330</v>
+        <v>84</v>
+      </c>
+      <c r="C81" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D82" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
+      <c r="B83" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="14" t="s">
-        <v>91</v>
-      </c>
+      <c r="B84" s="2"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="12" t="s">
-        <v>93</v>
+      <c r="B85" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C86" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>332</v>
-      </c>
+      <c r="B86" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B89" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C87" s="17" t="s">
+      <c r="C89" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B88" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C88" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C89" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>338</v>
+      <c r="D89" s="1" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B92" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C90" s="5" t="s">
+      <c r="C92" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B91" s="2" t="s">
+      <c r="D92" s="8" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C91" s="18" t="s">
+      <c r="C93" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D91" s="2"/>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B92" s="2" t="s">
+      <c r="D93" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B94" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C92" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="93" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B93" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C93" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="D93" s="2"/>
-    </row>
-    <row r="94" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B94" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C94" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="D94" s="2"/>
+      <c r="C94" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="D94" s="20" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="95" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C95" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B96" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C96" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B97" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C95" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B96" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C96" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D96" s="2"/>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C97" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="D97" s="2"/>
+      <c r="C97" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D98" s="2"/>
+        <v>104</v>
+      </c>
+      <c r="C98" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C99" s="5" t="s">
-        <v>121</v>
+        <v>105</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
+      <c r="B100" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="D100" s="2"/>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B101" s="14" t="s">
-        <v>122</v>
-      </c>
+      <c r="B101" s="2"/>
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B102" s="12" t="s">
-        <v>123</v>
+      <c r="B102" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B103" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C103" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>333</v>
-      </c>
+      <c r="B103" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C104" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="C104" s="17" t="s">
-        <v>129</v>
-      </c>
       <c r="D104" s="2" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C105" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="D105" s="2"/>
+      <c r="D105" s="2" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="106" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C106" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="D106" s="5" t="s">
-        <v>336</v>
-      </c>
+      <c r="D106" s="2"/>
     </row>
     <row r="107" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
+      <c r="B107" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C107" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B108" s="14" t="s">
-        <v>132</v>
-      </c>
+      <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>135</v>
-      </c>
+      <c r="B109" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="C109" s="2"/>
       <c r="D109" s="2"/>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C110" s="17" t="s">
-        <v>136</v>
+        <v>130</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="D110" s="2"/>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
+      <c r="B111" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B112" s="14" t="s">
-        <v>137</v>
-      </c>
+      <c r="B112" s="2"/>
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
     </row>
     <row r="113" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B113" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C113" s="17" t="s">
-        <v>25</v>
-      </c>
+      <c r="B113" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C113" s="2"/>
       <c r="D113" s="2"/>
     </row>
     <row r="114" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C114" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C114" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D114" s="2"/>
+      <c r="D114" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="115" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D115" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="116" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C116" s="5" t="s">
-        <v>154</v>
+        <v>137</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="D116" s="2"/>
     </row>
     <row r="117" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C117" s="17" t="s">
-        <v>155</v>
+        <v>138</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="D117" s="2"/>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C118" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="D118" s="2"/>
+        <v>139</v>
+      </c>
+      <c r="C118" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="119" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B119" t="s">
-        <v>144</v>
-      </c>
-      <c r="C119" s="19" t="s">
-        <v>157</v>
+      <c r="B119" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C119" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="120" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>145</v>
-      </c>
-      <c r="C120" s="19" t="s">
-        <v>158</v>
+        <v>141</v>
+      </c>
+      <c r="C120" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>146</v>
-      </c>
-      <c r="C121" t="s">
-        <v>84</v>
+        <v>142</v>
+      </c>
+      <c r="C121" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="D121" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="122" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>147</v>
-      </c>
-      <c r="C122" s="19" t="s">
-        <v>159</v>
+        <v>143</v>
+      </c>
+      <c r="C122" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="123" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>148</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>160</v>
+        <v>144</v>
+      </c>
+      <c r="C123" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D123" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="124" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>149</v>
-      </c>
-      <c r="C124" s="19" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B126" t="s">
-        <v>168</v>
-      </c>
-      <c r="C126" t="s">
-        <v>172</v>
+        <v>145</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>146</v>
+      </c>
+      <c r="C125" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D125" s="8" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="127" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
+        <v>162</v>
+      </c>
+      <c r="C127" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>163</v>
+      </c>
+      <c r="C128" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D128" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>164</v>
+      </c>
+      <c r="C129" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D129" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>160</v>
+      </c>
+      <c r="C130" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>165</v>
+      </c>
+      <c r="C131" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>161</v>
+      </c>
+      <c r="C132" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>147</v>
+      </c>
+      <c r="C135" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>148</v>
+      </c>
+      <c r="C136" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>149</v>
+      </c>
+      <c r="C137" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" s="6"/>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="C127" s="19" t="s">
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>170</v>
+      </c>
+      <c r="C140" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D140" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>171</v>
+      </c>
+      <c r="C141" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>172</v>
+      </c>
+      <c r="C142" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D142" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B128" t="s">
-        <v>170</v>
-      </c>
-      <c r="C128" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B129" t="s">
-        <v>166</v>
-      </c>
-      <c r="C129" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B130" t="s">
-        <v>171</v>
-      </c>
-      <c r="C130" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
-        <v>167</v>
-      </c>
-      <c r="C131" t="s">
+      <c r="C143" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B134" t="s">
-        <v>150</v>
-      </c>
-      <c r="C134" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B135" t="s">
-        <v>151</v>
-      </c>
-      <c r="C135" s="19" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
-        <v>152</v>
-      </c>
-      <c r="C136" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B137" s="7"/>
-    </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B138" s="11" t="s">
+      <c r="C144" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="D144" s="5"/>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B139" t="s">
-        <v>176</v>
-      </c>
-      <c r="C139" s="19" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B140" t="s">
-        <v>177</v>
-      </c>
-      <c r="C140" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
-        <v>178</v>
-      </c>
-      <c r="C141" s="19" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B142" t="s">
+      <c r="C145" t="s">
         <v>179</v>
       </c>
-      <c r="C142" s="19" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" s="10" t="s">
         <v>180</v>
-      </c>
-      <c r="C143" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
-        <v>181</v>
-      </c>
-      <c r="C144" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B146" s="11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B147" t="s">
-        <v>188</v>
-      </c>
-      <c r="C147" s="19" t="s">
-        <v>315</v>
-      </c>
-      <c r="D147" s="22" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>189</v>
-      </c>
-      <c r="C148" t="s">
-        <v>194</v>
+        <v>181</v>
+      </c>
+      <c r="C148" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="D148" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>190</v>
-      </c>
-      <c r="C149" s="19" t="s">
-        <v>23</v>
+        <v>182</v>
+      </c>
+      <c r="C149" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>191</v>
-      </c>
-      <c r="C150" s="19" t="s">
-        <v>195</v>
+        <v>183</v>
+      </c>
+      <c r="C150" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D150" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>192</v>
-      </c>
-      <c r="C151" s="6" t="s">
-        <v>154</v>
+        <v>184</v>
+      </c>
+      <c r="C151" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D151" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
+        <v>185</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>186</v>
+      </c>
+      <c r="C153" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>191</v>
+      </c>
+      <c r="C156" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="C152" t="s">
+      <c r="D156" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>192</v>
+      </c>
+      <c r="C157" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>193</v>
+      </c>
+      <c r="C158" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="D158" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>194</v>
+      </c>
+      <c r="C159" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>195</v>
+      </c>
+      <c r="C160" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B154" s="11" t="s">
+      <c r="C161" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="162" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="155" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B155" t="s">
+      <c r="C162" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D162" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
         <v>198</v>
       </c>
-      <c r="C155" s="19" t="s">
+      <c r="C163" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="164" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>199</v>
+      </c>
+      <c r="C164" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
         <v>200</v>
       </c>
-      <c r="D155" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B156" t="s">
-        <v>199</v>
-      </c>
-      <c r="C156" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="157" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B157" t="s">
-        <v>200</v>
-      </c>
-      <c r="C157" s="19" t="s">
+      <c r="C165" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="166" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>201</v>
+      </c>
+      <c r="C166" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="D157" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B158" t="s">
-        <v>201</v>
-      </c>
-      <c r="C158" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="159" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
-        <v>202</v>
-      </c>
-      <c r="C159" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="D159" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B160" t="s">
-        <v>203</v>
-      </c>
-      <c r="C160" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="161" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B161" t="s">
-        <v>204</v>
-      </c>
-      <c r="C161" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="162" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B162" t="s">
-        <v>205</v>
-      </c>
-      <c r="C162" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="163" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B163" t="s">
-        <v>206</v>
-      </c>
-      <c r="C163" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="164" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B164" t="s">
-        <v>207</v>
-      </c>
-      <c r="C164" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="165" spans="2:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B165" t="s">
-        <v>208</v>
-      </c>
-      <c r="C165" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="D165" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="166" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B166" t="s">
-        <v>119</v>
-      </c>
-      <c r="C166" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="167" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="D166" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>209</v>
-      </c>
-      <c r="C167" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C167" t="s">
         <v>210</v>
-      </c>
-      <c r="D167" s="1" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="168" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>210</v>
-      </c>
-      <c r="C168" s="19" t="s">
-        <v>218</v>
+        <v>202</v>
+      </c>
+      <c r="C168" s="17" t="s">
+        <v>203</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B170" s="11" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="171" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="169" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>203</v>
+      </c>
+      <c r="C169" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B171" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C171" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="D171" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="172" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B172" t="s">
-        <v>221</v>
-      </c>
-      <c r="C172" t="s">
-        <v>224</v>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="172" spans="2:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B172" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C172" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="173" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C173" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B175" s="11" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="176" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B176" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>215</v>
+      </c>
+      <c r="C174" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B176" s="10" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="177" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B177" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C177" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B178" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C178" s="20" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B180" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B181" s="12" t="s">
         <v>226</v>
-      </c>
-      <c r="C176" s="9" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="177" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B177" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C177" s="23" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="179" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B179" s="11" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="180" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B180" s="13" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="181" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B181" t="s">
-        <v>229</v>
-      </c>
-      <c r="C181" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="182" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="C182" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B184" s="13" t="s">
-        <v>234</v>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
+        <v>223</v>
+      </c>
+      <c r="C183" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="185" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B185" t="s">
-        <v>235</v>
-      </c>
-      <c r="C185" t="s">
-        <v>239</v>
+      <c r="B185" s="12" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="186" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>236</v>
-      </c>
-      <c r="C186" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="D186" t="s">
-        <v>339</v>
+        <v>228</v>
+      </c>
+      <c r="C186" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="187" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>237</v>
-      </c>
-      <c r="C187" t="s">
-        <v>240</v>
+        <v>229</v>
+      </c>
+      <c r="C187" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="D187" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="188" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>238</v>
-      </c>
-      <c r="C188" s="19" t="s">
-        <v>242</v>
-      </c>
-      <c r="D188" s="24"/>
-    </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B190" s="11" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B192" s="13" t="s">
-        <v>244</v>
+        <v>230</v>
+      </c>
+      <c r="C188" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="189" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
+        <v>231</v>
+      </c>
+      <c r="C189" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D189" s="8" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B191" s="10" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="193" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B193" t="s">
-        <v>246</v>
-      </c>
-      <c r="C193" t="s">
-        <v>248</v>
+      <c r="B193" s="12" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="194" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>247</v>
-      </c>
-      <c r="C194" s="19" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B196" s="13" t="s">
-        <v>245</v>
+        <v>239</v>
+      </c>
+      <c r="C194" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>240</v>
+      </c>
+      <c r="C195" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="D195" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="197" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B197" t="s">
-        <v>250</v>
-      </c>
-      <c r="C197" t="s">
-        <v>252</v>
+      <c r="B197" s="12" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="198" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="C198" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B200" s="13" t="s">
-        <v>254</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>244</v>
+      </c>
+      <c r="C199" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="201" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B201" t="s">
-        <v>255</v>
-      </c>
-      <c r="C201" t="s">
-        <v>259</v>
+      <c r="B201" s="12" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="202" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C202" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="203" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>257</v>
-      </c>
-      <c r="C203" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="D203" t="s">
-        <v>340</v>
+        <v>249</v>
+      </c>
+      <c r="C203" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="204" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>258</v>
-      </c>
-      <c r="C204" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B206" s="11" t="s">
-        <v>263</v>
+        <v>250</v>
+      </c>
+      <c r="C204" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="D204" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
+        <v>251</v>
+      </c>
+      <c r="C205" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="207" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B207" s="8"/>
+      <c r="B207" s="10" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="208" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B208" s="13" t="s">
-        <v>264</v>
-      </c>
+      <c r="B208" s="7"/>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B209" t="s">
-        <v>266</v>
-      </c>
-      <c r="C209" t="s">
-        <v>269</v>
+      <c r="B209" s="12" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="C210" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
+        <v>260</v>
+      </c>
+      <c r="C211" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>261</v>
+      </c>
+      <c r="C212" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B214" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
+        <v>265</v>
+      </c>
+      <c r="C215" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B217" s="10" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
         <v>268</v>
       </c>
-      <c r="C211" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B213" s="13" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B214" t="s">
-        <v>272</v>
-      </c>
-      <c r="C214" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B216" s="11" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B217" t="s">
-        <v>275</v>
-      </c>
-      <c r="C217" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B219" s="11" t="s">
-        <v>277</v>
+      <c r="C218" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B220" t="s">
-        <v>278</v>
-      </c>
-      <c r="C220" t="s">
-        <v>283</v>
+      <c r="B220" s="10" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="C221" t="s">
-        <v>41</v>
+        <v>276</v>
       </c>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C222" t="s">
-        <v>284</v>
+        <v>40</v>
       </c>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C223" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C224" t="s">
-        <v>286</v>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>275</v>
+      </c>
+      <c r="C225" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>